<commit_message>
chot csdl lan 2
</commit_message>
<xml_diff>
--- a/database/seeders/_lop_hoc_seeder.xlsx
+++ b/database/seeders/_lop_hoc_seeder.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>9:00:00</t>
   </si>
@@ -64,15 +64,9 @@
     <t>hoc_sinh_id</t>
   </si>
   <si>
-    <t>daketthuc</t>
-  </si>
-  <si>
     <t>HP-TGVV-0001</t>
   </si>
   <si>
-    <t>danghoatdong</t>
-  </si>
-  <si>
     <t>HP-XCTRB-0001</t>
   </si>
   <si>
@@ -89,6 +83,30 @@
   </si>
   <si>
     <t>tenlop</t>
+  </si>
+  <si>
+    <t>Đang hoạt động</t>
+  </si>
+  <si>
+    <t>Đã kết thúc</t>
+  </si>
+  <si>
+    <t>2020/05/07</t>
+  </si>
+  <si>
+    <t>2020/07/07</t>
+  </si>
+  <si>
+    <t>2020/06/08</t>
+  </si>
+  <si>
+    <t>2020/08/15</t>
+  </si>
+  <si>
+    <t>ngaybatdau</t>
+  </si>
+  <si>
+    <t>ngayketthuc</t>
   </si>
 </sst>
 </file>
@@ -431,63 +449,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="3" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
         <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
+      <c r="F3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Them tim kiem lop hoc theo khoa hoc
</commit_message>
<xml_diff>
--- a/database/seeders/_lop_hoc_seeder.xlsx
+++ b/database/seeders/_lop_hoc_seeder.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
   <si>
     <t>11:30:00</t>
   </si>
@@ -110,12 +110,6 @@
   </si>
   <si>
     <t>MNCN-LTVS-5/10/2020</t>
-  </si>
-  <si>
-    <t>BLG-C1-2/10/2020</t>
-  </si>
-  <si>
-    <t>MNCN-LTVS-10/10/2020</t>
   </si>
   <si>
     <t>MNCN-LTVS-17/10/2020</t>
@@ -537,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,7 +556,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>13</v>
@@ -574,10 +568,10 @@
         <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>12</v>
@@ -592,7 +586,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -600,7 +594,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>17</v>
@@ -648,14 +642,14 @@
         <v>43990</v>
       </c>
       <c r="E3" s="6">
-        <f t="shared" ref="E3:E19" si="0">(D3+70)</f>
+        <f t="shared" ref="E3:E17" si="0">(D3+70)</f>
         <v>44060</v>
       </c>
       <c r="F3" s="2">
         <v>10</v>
       </c>
       <c r="G3" s="7">
-        <f t="shared" ref="G3:G19" ca="1" si="1">TODAY()-D3</f>
+        <f t="shared" ref="G3:G17" ca="1" si="1">TODAY()-D3</f>
         <v>166</v>
       </c>
       <c r="H3" s="5"/>
@@ -669,7 +663,7 @@
       <c r="L3" s="4"/>
       <c r="M3" s="2"/>
       <c r="N3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -707,7 +701,7 @@
       <c r="L4" s="4"/>
       <c r="M4" s="2"/>
       <c r="N4" s="1">
-        <f t="shared" ref="N3:N19" ca="1" si="2">QUOTIENT(G4,7)</f>
+        <f t="shared" ref="N4:N17" ca="1" si="2">QUOTIENT(G4,7)</f>
         <v>7</v>
       </c>
     </row>
@@ -791,85 +785,85 @@
     </row>
     <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="7">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="6">
-        <v>44114</v>
+        <v>44121</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>44184</v>
+        <v>44191</v>
       </c>
       <c r="F7" s="2">
         <v>10</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="2">
         <v>1</v>
       </c>
       <c r="J7" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="7">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="6">
-        <v>44121</v>
+        <v>44141</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" si="0"/>
-        <v>44191</v>
+        <v>44211</v>
       </c>
       <c r="F8" s="2">
         <v>10</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="2">
-        <v>7</v>
-      </c>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
@@ -878,37 +872,37 @@
         <v>17</v>
       </c>
       <c r="D9" s="6">
-        <v>44106</v>
+        <v>44148</v>
       </c>
       <c r="E9" s="6">
         <f t="shared" si="0"/>
-        <v>44176</v>
+        <v>44218</v>
       </c>
       <c r="F9" s="2">
         <v>10</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="2">
         <v>2</v>
       </c>
       <c r="J9" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="7">
         <v>0</v>
@@ -917,37 +911,37 @@
         <v>17</v>
       </c>
       <c r="D10" s="6">
-        <v>44141</v>
+        <v>44132</v>
       </c>
       <c r="E10" s="6">
         <f t="shared" si="0"/>
-        <v>44211</v>
+        <v>44202</v>
       </c>
       <c r="F10" s="2">
         <v>10</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="2">
         <v>2</v>
       </c>
       <c r="J10" s="2">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B11" s="7">
         <v>0</v>
@@ -956,25 +950,25 @@
         <v>17</v>
       </c>
       <c r="D11" s="6">
-        <v>44148</v>
+        <v>44145</v>
       </c>
       <c r="E11" s="6">
         <f t="shared" si="0"/>
-        <v>44218</v>
+        <v>44215</v>
       </c>
       <c r="F11" s="2">
         <v>10</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="2">
         <v>2</v>
       </c>
       <c r="J11" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -986,7 +980,7 @@
     </row>
     <row r="12" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B12" s="7">
         <v>0</v>
@@ -995,37 +989,37 @@
         <v>17</v>
       </c>
       <c r="D12" s="6">
-        <v>44132</v>
+        <v>44146</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" si="0"/>
-        <v>44202</v>
+        <v>44216</v>
       </c>
       <c r="F12" s="2">
         <v>10</v>
       </c>
       <c r="G12" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="2">
         <v>2</v>
       </c>
       <c r="J12" s="2">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="7">
         <v>0</v>
@@ -1034,37 +1028,37 @@
         <v>17</v>
       </c>
       <c r="D13" s="6">
-        <v>44145</v>
+        <v>44112</v>
       </c>
       <c r="E13" s="6">
         <f t="shared" si="0"/>
-        <v>44215</v>
+        <v>44182</v>
       </c>
       <c r="F13" s="2">
         <v>10</v>
       </c>
       <c r="G13" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J13" s="2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B14" s="7">
         <v>0</v>
@@ -1073,32 +1067,32 @@
         <v>17</v>
       </c>
       <c r="D14" s="6">
-        <v>44146</v>
+        <v>44116</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" si="0"/>
-        <v>44216</v>
+        <v>44186</v>
       </c>
       <c r="F14" s="2">
         <v>10</v>
       </c>
       <c r="G14" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" s="2">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -1112,32 +1106,32 @@
         <v>17</v>
       </c>
       <c r="D15" s="6">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="E15" s="6">
         <f t="shared" si="0"/>
-        <v>44182</v>
+        <v>44190</v>
       </c>
       <c r="F15" s="2">
         <v>10</v>
       </c>
       <c r="G15" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="2">
         <v>3</v>
       </c>
       <c r="J15" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -1151,32 +1145,32 @@
         <v>17</v>
       </c>
       <c r="D16" s="6">
-        <v>44116</v>
+        <v>44125</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" si="0"/>
-        <v>44186</v>
+        <v>44195</v>
       </c>
       <c r="F16" s="2">
         <v>10</v>
       </c>
       <c r="G16" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="2">
         <v>3</v>
       </c>
       <c r="J16" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
@@ -1190,117 +1184,39 @@
         <v>17</v>
       </c>
       <c r="D17" s="6">
-        <v>44120</v>
+        <v>44129</v>
       </c>
       <c r="E17" s="6">
         <f t="shared" si="0"/>
-        <v>44190</v>
+        <v>44199</v>
       </c>
       <c r="F17" s="2">
         <v>10</v>
       </c>
       <c r="G17" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="2">
         <v>3</v>
       </c>
       <c r="J17" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="7">
-        <v>0</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="6">
-        <v>44125</v>
-      </c>
-      <c r="E18" s="6">
-        <f t="shared" si="0"/>
-        <v>44195</v>
-      </c>
-      <c r="F18" s="2">
-        <v>10</v>
-      </c>
-      <c r="G18" s="7">
-        <f t="shared" ca="1" si="1"/>
-        <v>31</v>
-      </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="2">
         <v>3</v>
       </c>
-      <c r="J18" s="2">
-        <v>17</v>
-      </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" s="7">
-        <v>0</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="6">
-        <v>44129</v>
-      </c>
-      <c r="E19" s="6">
-        <f t="shared" si="0"/>
-        <v>44199</v>
-      </c>
-      <c r="F19" s="2">
-        <v>10</v>
-      </c>
-      <c r="G19" s="7">
-        <f t="shared" ca="1" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="H19" s="5"/>
-      <c r="I19" s="2">
-        <v>3</v>
-      </c>
-      <c r="J19" s="2">
-        <v>17</v>
-      </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
linh vuc hoc vien
</commit_message>
<xml_diff>
--- a/database/seeders/_lop_hoc_seeder.xlsx
+++ b/database/seeders/_lop_hoc_seeder.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22E639C-E85B-4AEB-BD80-D3D9883754D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15132" windowHeight="4872" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="lop_hoc" sheetId="5" r:id="rId1"/>
     <sheet name="ca_hoc" sheetId="2" r:id="rId2"/>
     <sheet name="thoi_gian_hoc" sheetId="3" r:id="rId3"/>
     <sheet name="phan_lop" sheetId="4" r:id="rId4"/>
+    <sheet name="linh_vuc" sheetId="6" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>11:30:00</t>
   </si>
@@ -161,19 +163,29 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>loai_khoa_hoc_id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <sz val="10"/>
@@ -220,33 +232,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{DA1F8502-EF46-4B57-BC2A-16F22D5F11F0}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -337,6 +354,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -372,6 +406,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -547,28 +598,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="12.25" customWidth="1"/>
+    <col min="14" max="14" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -606,7 +657,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -628,7 +679,7 @@
       </c>
       <c r="G2" s="6">
         <f ca="1">TODAY()-D2</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="2">
@@ -642,10 +693,10 @@
       <c r="M2" s="2"/>
       <c r="N2" s="1">
         <f ca="1">QUOTIENT(G2,7)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -667,7 +718,7 @@
       </c>
       <c r="G3" s="6">
         <f t="shared" ref="G3:G17" ca="1" si="1">TODAY()-D3</f>
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="2">
@@ -683,7 +734,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -705,7 +756,7 @@
       </c>
       <c r="G4" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="2">
@@ -722,7 +773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>29</v>
       </c>
@@ -744,7 +795,7 @@
       </c>
       <c r="G5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="2">
@@ -761,7 +812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>30</v>
       </c>
@@ -783,7 +834,7 @@
       </c>
       <c r="G6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="2">
@@ -800,7 +851,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -822,7 +873,7 @@
       </c>
       <c r="G7" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="2">
@@ -839,7 +890,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
@@ -861,7 +912,7 @@
       </c>
       <c r="G8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="2">
@@ -878,7 +929,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>43</v>
       </c>
@@ -900,7 +951,7 @@
       </c>
       <c r="G9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="2">
@@ -917,7 +968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -939,7 +990,7 @@
       </c>
       <c r="G10" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="2">
@@ -953,10 +1004,10 @@
       <c r="M10" s="2"/>
       <c r="N10" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>34</v>
       </c>
@@ -978,7 +1029,7 @@
       </c>
       <c r="G11" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="2">
@@ -995,7 +1046,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
@@ -1017,7 +1068,7 @@
       </c>
       <c r="G12" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="2">
@@ -1031,10 +1082,10 @@
       <c r="M12" s="2"/>
       <c r="N12" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
@@ -1056,7 +1107,7 @@
       </c>
       <c r="G13" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="2">
@@ -1073,7 +1124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1095,7 +1146,7 @@
       </c>
       <c r="G14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="2">
@@ -1112,7 +1163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1134,7 +1185,7 @@
       </c>
       <c r="G15" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="2">
@@ -1151,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>38</v>
       </c>
@@ -1173,7 +1224,7 @@
       </c>
       <c r="G16" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="2">
@@ -1187,10 +1238,10 @@
       <c r="M16" s="2"/>
       <c r="N16" s="1">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>39</v>
       </c>
@@ -1212,7 +1263,7 @@
       </c>
       <c r="G17" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="2">
@@ -1229,7 +1280,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1245,7 +1296,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="1"/>
     </row>
-    <row r="19" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="6"/>
       <c r="C19" s="2"/>
@@ -1268,20 +1319,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1292,7 +1343,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1303,7 +1354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -1314,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1325,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1336,7 +1387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>22</v>
       </c>
@@ -1347,7 +1398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -1358,11 +1409,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
     </row>
@@ -1372,21 +1423,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="21.875" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1400,7 +1451,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1414,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1428,7 +1479,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1442,7 +1493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1456,7 +1507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1470,7 +1521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1484,7 +1535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1498,7 +1549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1512,7 +1563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1526,7 +1577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1540,7 +1591,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1554,7 +1605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1568,7 +1619,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1582,7 +1633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1596,7 +1647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1610,7 +1661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1630,20 +1681,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="A32:C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1651,7 +1702,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1</v>
       </c>
@@ -1659,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>2</v>
       </c>
@@ -1667,7 +1718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>3</v>
       </c>
@@ -1675,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>4</v>
       </c>
@@ -1683,7 +1734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>5</v>
       </c>
@@ -1691,7 +1742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>6</v>
       </c>
@@ -1699,7 +1750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>7</v>
       </c>
@@ -1707,7 +1758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -1715,7 +1766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>59</v>
       </c>
@@ -1723,7 +1774,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>60</v>
       </c>
@@ -1731,7 +1782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>57</v>
       </c>
@@ -1739,7 +1790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>58</v>
       </c>
@@ -1747,7 +1798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>55</v>
       </c>
@@ -1755,7 +1806,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>56</v>
       </c>
@@ -1763,7 +1814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>53</v>
       </c>
@@ -1771,7 +1822,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>54</v>
       </c>
@@ -1779,7 +1830,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>51</v>
       </c>
@@ -1787,7 +1838,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>52</v>
       </c>
@@ -1795,7 +1846,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>49</v>
       </c>
@@ -1803,7 +1854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>50</v>
       </c>
@@ -1811,7 +1862,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>47</v>
       </c>
@@ -1819,7 +1870,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>48</v>
       </c>
@@ -1827,7 +1878,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>45</v>
       </c>
@@ -1835,7 +1886,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>46</v>
       </c>
@@ -1843,7 +1894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>43</v>
       </c>
@@ -1851,7 +1902,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>44</v>
       </c>
@@ -1859,7 +1910,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>41</v>
       </c>
@@ -1867,7 +1918,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>42</v>
       </c>
@@ -1875,7 +1926,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>36</v>
       </c>
@@ -1883,7 +1934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>37</v>
       </c>
@@ -1891,17 +1942,932 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
     </row>
-    <row r="34" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{267E962A-9ECE-4AD8-A039-1813170F9752}">
+  <dimension ref="A1:XFD49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="252" width="9" style="8"/>
+    <col min="253" max="16380" width="9" style="9"/>
+    <col min="16381" max="16384" width="9" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:252" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>8</v>
+      </c>
+      <c r="B2" s="9">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
+      <c r="BN2" s="8"/>
+      <c r="BO2" s="8"/>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="8"/>
+      <c r="BZ2" s="8"/>
+      <c r="CA2" s="8"/>
+      <c r="CB2" s="8"/>
+      <c r="CC2" s="8"/>
+      <c r="CD2" s="8"/>
+      <c r="CE2" s="8"/>
+      <c r="CF2" s="8"/>
+      <c r="CG2" s="8"/>
+      <c r="CH2" s="8"/>
+      <c r="CI2" s="8"/>
+      <c r="CJ2" s="8"/>
+      <c r="CK2" s="8"/>
+      <c r="CL2" s="8"/>
+      <c r="CM2" s="8"/>
+      <c r="CN2" s="8"/>
+      <c r="CO2" s="8"/>
+      <c r="CP2" s="8"/>
+      <c r="CQ2" s="8"/>
+      <c r="CR2" s="8"/>
+      <c r="CS2" s="8"/>
+      <c r="CT2" s="8"/>
+      <c r="CU2" s="8"/>
+      <c r="CV2" s="8"/>
+      <c r="CW2" s="8"/>
+      <c r="CX2" s="8"/>
+      <c r="CY2" s="8"/>
+      <c r="CZ2" s="8"/>
+      <c r="DA2" s="8"/>
+      <c r="DB2" s="8"/>
+      <c r="DC2" s="8"/>
+      <c r="DD2" s="8"/>
+      <c r="DE2" s="8"/>
+      <c r="DF2" s="8"/>
+      <c r="DG2" s="8"/>
+      <c r="DH2" s="8"/>
+      <c r="DI2" s="8"/>
+      <c r="DJ2" s="8"/>
+      <c r="DK2" s="8"/>
+      <c r="DL2" s="8"/>
+      <c r="DM2" s="8"/>
+      <c r="DN2" s="8"/>
+      <c r="DO2" s="8"/>
+      <c r="DP2" s="8"/>
+      <c r="DQ2" s="8"/>
+      <c r="DR2" s="8"/>
+      <c r="DS2" s="8"/>
+      <c r="DT2" s="8"/>
+      <c r="DU2" s="8"/>
+      <c r="DV2" s="8"/>
+      <c r="DW2" s="8"/>
+      <c r="DX2" s="8"/>
+      <c r="DY2" s="8"/>
+      <c r="DZ2" s="8"/>
+      <c r="EA2" s="8"/>
+      <c r="EB2" s="8"/>
+      <c r="EC2" s="8"/>
+      <c r="ED2" s="8"/>
+      <c r="EE2" s="8"/>
+      <c r="EF2" s="8"/>
+      <c r="EG2" s="8"/>
+      <c r="EH2" s="8"/>
+      <c r="EI2" s="8"/>
+      <c r="EJ2" s="8"/>
+      <c r="EK2" s="8"/>
+      <c r="EL2" s="8"/>
+      <c r="EM2" s="8"/>
+      <c r="EN2" s="8"/>
+      <c r="EO2" s="8"/>
+      <c r="EP2" s="8"/>
+      <c r="EQ2" s="8"/>
+      <c r="ER2" s="8"/>
+      <c r="ES2" s="8"/>
+      <c r="ET2" s="8"/>
+      <c r="EU2" s="8"/>
+      <c r="EV2" s="8"/>
+      <c r="EW2" s="8"/>
+      <c r="EX2" s="8"/>
+      <c r="EY2" s="8"/>
+      <c r="EZ2" s="8"/>
+      <c r="FA2" s="8"/>
+      <c r="FB2" s="8"/>
+      <c r="FC2" s="8"/>
+      <c r="FD2" s="8"/>
+      <c r="FE2" s="8"/>
+      <c r="FF2" s="8"/>
+      <c r="FG2" s="8"/>
+      <c r="FH2" s="8"/>
+      <c r="FI2" s="8"/>
+      <c r="FJ2" s="8"/>
+      <c r="FK2" s="8"/>
+      <c r="FL2" s="8"/>
+      <c r="FM2" s="8"/>
+      <c r="FN2" s="8"/>
+      <c r="FO2" s="8"/>
+      <c r="FP2" s="8"/>
+      <c r="FQ2" s="8"/>
+      <c r="FR2" s="8"/>
+      <c r="FS2" s="8"/>
+      <c r="FT2" s="8"/>
+      <c r="FU2" s="8"/>
+      <c r="FV2" s="8"/>
+      <c r="FW2" s="8"/>
+      <c r="FX2" s="8"/>
+      <c r="FY2" s="8"/>
+      <c r="FZ2" s="8"/>
+      <c r="GA2" s="8"/>
+      <c r="GB2" s="8"/>
+      <c r="GC2" s="8"/>
+      <c r="GD2" s="8"/>
+      <c r="GE2" s="8"/>
+      <c r="GF2" s="8"/>
+      <c r="GG2" s="8"/>
+      <c r="GH2" s="8"/>
+      <c r="GI2" s="8"/>
+      <c r="GJ2" s="8"/>
+      <c r="GK2" s="8"/>
+      <c r="GL2" s="8"/>
+      <c r="GM2" s="8"/>
+      <c r="GN2" s="8"/>
+      <c r="GO2" s="8"/>
+      <c r="GP2" s="8"/>
+      <c r="GQ2" s="8"/>
+      <c r="GR2" s="8"/>
+      <c r="GS2" s="8"/>
+      <c r="GT2" s="8"/>
+      <c r="GU2" s="8"/>
+      <c r="GV2" s="8"/>
+      <c r="GW2" s="8"/>
+      <c r="GX2" s="8"/>
+      <c r="GY2" s="8"/>
+      <c r="GZ2" s="8"/>
+      <c r="HA2" s="8"/>
+      <c r="HB2" s="8"/>
+      <c r="HC2" s="8"/>
+      <c r="HD2" s="8"/>
+      <c r="HE2" s="8"/>
+      <c r="HF2" s="8"/>
+      <c r="HG2" s="8"/>
+      <c r="HH2" s="8"/>
+      <c r="HI2" s="8"/>
+      <c r="HJ2" s="8"/>
+      <c r="HK2" s="8"/>
+      <c r="HL2" s="8"/>
+      <c r="HM2" s="8"/>
+      <c r="HN2" s="8"/>
+      <c r="HO2" s="8"/>
+      <c r="HP2" s="8"/>
+      <c r="HQ2" s="8"/>
+      <c r="HR2" s="8"/>
+      <c r="HS2" s="8"/>
+      <c r="HT2" s="8"/>
+      <c r="HU2" s="8"/>
+      <c r="HV2" s="8"/>
+      <c r="HW2" s="8"/>
+      <c r="HX2" s="8"/>
+      <c r="HY2" s="8"/>
+      <c r="HZ2" s="8"/>
+      <c r="IA2" s="8"/>
+      <c r="IB2" s="8"/>
+      <c r="IC2" s="8"/>
+      <c r="ID2" s="8"/>
+      <c r="IE2" s="8"/>
+      <c r="IF2" s="8"/>
+      <c r="IG2" s="8"/>
+      <c r="IH2" s="8"/>
+      <c r="II2" s="8"/>
+      <c r="IJ2" s="8"/>
+      <c r="IK2" s="8"/>
+      <c r="IL2" s="8"/>
+      <c r="IM2" s="8"/>
+      <c r="IN2" s="8"/>
+      <c r="IO2" s="8"/>
+      <c r="IP2" s="8"/>
+      <c r="IQ2" s="8"/>
+      <c r="IR2" s="8"/>
+    </row>
+    <row r="3" spans="1:252" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
+        <v>29</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="8"/>
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+      <c r="BG3" s="8"/>
+      <c r="BH3" s="8"/>
+      <c r="BI3" s="8"/>
+      <c r="BJ3" s="8"/>
+      <c r="BK3" s="8"/>
+      <c r="BL3" s="8"/>
+      <c r="BM3" s="8"/>
+      <c r="BN3" s="8"/>
+      <c r="BO3" s="8"/>
+      <c r="BP3" s="8"/>
+      <c r="BQ3" s="8"/>
+      <c r="BR3" s="8"/>
+      <c r="BS3" s="8"/>
+      <c r="BT3" s="8"/>
+      <c r="BU3" s="8"/>
+      <c r="BV3" s="8"/>
+      <c r="BW3" s="8"/>
+      <c r="BX3" s="8"/>
+      <c r="BY3" s="8"/>
+      <c r="BZ3" s="8"/>
+      <c r="CA3" s="8"/>
+      <c r="CB3" s="8"/>
+      <c r="CC3" s="8"/>
+      <c r="CD3" s="8"/>
+      <c r="CE3" s="8"/>
+      <c r="CF3" s="8"/>
+      <c r="CG3" s="8"/>
+      <c r="CH3" s="8"/>
+      <c r="CI3" s="8"/>
+      <c r="CJ3" s="8"/>
+      <c r="CK3" s="8"/>
+      <c r="CL3" s="8"/>
+      <c r="CM3" s="8"/>
+      <c r="CN3" s="8"/>
+      <c r="CO3" s="8"/>
+      <c r="CP3" s="8"/>
+      <c r="CQ3" s="8"/>
+      <c r="CR3" s="8"/>
+      <c r="CS3" s="8"/>
+      <c r="CT3" s="8"/>
+      <c r="CU3" s="8"/>
+      <c r="CV3" s="8"/>
+      <c r="CW3" s="8"/>
+      <c r="CX3" s="8"/>
+      <c r="CY3" s="8"/>
+      <c r="CZ3" s="8"/>
+      <c r="DA3" s="8"/>
+      <c r="DB3" s="8"/>
+      <c r="DC3" s="8"/>
+      <c r="DD3" s="8"/>
+      <c r="DE3" s="8"/>
+      <c r="DF3" s="8"/>
+      <c r="DG3" s="8"/>
+      <c r="DH3" s="8"/>
+      <c r="DI3" s="8"/>
+      <c r="DJ3" s="8"/>
+      <c r="DK3" s="8"/>
+      <c r="DL3" s="8"/>
+      <c r="DM3" s="8"/>
+      <c r="DN3" s="8"/>
+      <c r="DO3" s="8"/>
+      <c r="DP3" s="8"/>
+      <c r="DQ3" s="8"/>
+      <c r="DR3" s="8"/>
+      <c r="DS3" s="8"/>
+      <c r="DT3" s="8"/>
+      <c r="DU3" s="8"/>
+      <c r="DV3" s="8"/>
+      <c r="DW3" s="8"/>
+      <c r="DX3" s="8"/>
+      <c r="DY3" s="8"/>
+      <c r="DZ3" s="8"/>
+      <c r="EA3" s="8"/>
+      <c r="EB3" s="8"/>
+      <c r="EC3" s="8"/>
+      <c r="ED3" s="8"/>
+      <c r="EE3" s="8"/>
+      <c r="EF3" s="8"/>
+      <c r="EG3" s="8"/>
+      <c r="EH3" s="8"/>
+      <c r="EI3" s="8"/>
+      <c r="EJ3" s="8"/>
+      <c r="EK3" s="8"/>
+      <c r="EL3" s="8"/>
+      <c r="EM3" s="8"/>
+      <c r="EN3" s="8"/>
+      <c r="EO3" s="8"/>
+      <c r="EP3" s="8"/>
+      <c r="EQ3" s="8"/>
+      <c r="ER3" s="8"/>
+      <c r="ES3" s="8"/>
+      <c r="ET3" s="8"/>
+      <c r="EU3" s="8"/>
+      <c r="EV3" s="8"/>
+      <c r="EW3" s="8"/>
+      <c r="EX3" s="8"/>
+      <c r="EY3" s="8"/>
+      <c r="EZ3" s="8"/>
+      <c r="FA3" s="8"/>
+      <c r="FB3" s="8"/>
+      <c r="FC3" s="8"/>
+      <c r="FD3" s="8"/>
+      <c r="FE3" s="8"/>
+      <c r="FF3" s="8"/>
+      <c r="FG3" s="8"/>
+      <c r="FH3" s="8"/>
+      <c r="FI3" s="8"/>
+      <c r="FJ3" s="8"/>
+      <c r="FK3" s="8"/>
+      <c r="FL3" s="8"/>
+      <c r="FM3" s="8"/>
+      <c r="FN3" s="8"/>
+      <c r="FO3" s="8"/>
+      <c r="FP3" s="8"/>
+      <c r="FQ3" s="8"/>
+      <c r="FR3" s="8"/>
+      <c r="FS3" s="8"/>
+      <c r="FT3" s="8"/>
+      <c r="FU3" s="8"/>
+      <c r="FV3" s="8"/>
+      <c r="FW3" s="8"/>
+      <c r="FX3" s="8"/>
+      <c r="FY3" s="8"/>
+      <c r="FZ3" s="8"/>
+      <c r="GA3" s="8"/>
+      <c r="GB3" s="8"/>
+      <c r="GC3" s="8"/>
+      <c r="GD3" s="8"/>
+      <c r="GE3" s="8"/>
+      <c r="GF3" s="8"/>
+      <c r="GG3" s="8"/>
+      <c r="GH3" s="8"/>
+      <c r="GI3" s="8"/>
+      <c r="GJ3" s="8"/>
+      <c r="GK3" s="8"/>
+      <c r="GL3" s="8"/>
+      <c r="GM3" s="8"/>
+      <c r="GN3" s="8"/>
+      <c r="GO3" s="8"/>
+      <c r="GP3" s="8"/>
+      <c r="GQ3" s="8"/>
+      <c r="GR3" s="8"/>
+      <c r="GS3" s="8"/>
+      <c r="GT3" s="8"/>
+      <c r="GU3" s="8"/>
+      <c r="GV3" s="8"/>
+      <c r="GW3" s="8"/>
+      <c r="GX3" s="8"/>
+      <c r="GY3" s="8"/>
+      <c r="GZ3" s="8"/>
+      <c r="HA3" s="8"/>
+      <c r="HB3" s="8"/>
+      <c r="HC3" s="8"/>
+      <c r="HD3" s="8"/>
+      <c r="HE3" s="8"/>
+      <c r="HF3" s="8"/>
+      <c r="HG3" s="8"/>
+      <c r="HH3" s="8"/>
+      <c r="HI3" s="8"/>
+      <c r="HJ3" s="8"/>
+      <c r="HK3" s="8"/>
+      <c r="HL3" s="8"/>
+      <c r="HM3" s="8"/>
+      <c r="HN3" s="8"/>
+      <c r="HO3" s="8"/>
+      <c r="HP3" s="8"/>
+      <c r="HQ3" s="8"/>
+      <c r="HR3" s="8"/>
+      <c r="HS3" s="8"/>
+      <c r="HT3" s="8"/>
+      <c r="HU3" s="8"/>
+      <c r="HV3" s="8"/>
+      <c r="HW3" s="8"/>
+      <c r="HX3" s="8"/>
+      <c r="HY3" s="8"/>
+      <c r="HZ3" s="8"/>
+      <c r="IA3" s="8"/>
+      <c r="IB3" s="8"/>
+      <c r="IC3" s="8"/>
+      <c r="ID3" s="8"/>
+      <c r="IE3" s="8"/>
+      <c r="IF3" s="8"/>
+      <c r="IG3" s="8"/>
+      <c r="IH3" s="8"/>
+      <c r="II3" s="8"/>
+      <c r="IJ3" s="8"/>
+      <c r="IK3" s="8"/>
+      <c r="IL3" s="8"/>
+      <c r="IM3" s="8"/>
+      <c r="IN3" s="8"/>
+      <c r="IO3" s="8"/>
+      <c r="IP3" s="8"/>
+      <c r="IQ3" s="8"/>
+      <c r="IR3" s="8"/>
+    </row>
+    <row r="4" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A4" s="8">
+        <v>8</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>1</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A6" s="8">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <v>5</v>
+      </c>
+      <c r="B9" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
+        <v>6</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <v>7</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A12" s="8">
+        <v>8</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A13" s="8">
+        <v>9</v>
+      </c>
+      <c r="B13" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <v>10</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <v>11</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:252" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
+        <v>12</v>
+      </c>
+      <c r="B16" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="8">
+        <v>14</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="8">
+        <v>15</v>
+      </c>
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="8">
+        <v>16</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>17</v>
+      </c>
+      <c r="B21" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="8">
+        <v>18</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <v>19</v>
+      </c>
+      <c r="B23" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="8">
+        <v>20</v>
+      </c>
+      <c r="B24" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="8">
+        <v>21</v>
+      </c>
+      <c r="B25" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="8">
+        <v>22</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="8">
+        <v>23</v>
+      </c>
+      <c r="B27" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="8">
+        <v>24</v>
+      </c>
+      <c r="B28" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="8">
+        <v>25</v>
+      </c>
+      <c r="B29" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="8">
+        <v>26</v>
+      </c>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="8">
+        <v>27</v>
+      </c>
+      <c r="B31" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="8">
+        <v>28</v>
+      </c>
+      <c r="B32" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="8">
+        <v>29</v>
+      </c>
+      <c r="B33" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="8">
+        <v>30</v>
+      </c>
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="8">
+        <v>31</v>
+      </c>
+      <c r="B35" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="8">
+        <v>32</v>
+      </c>
+      <c r="B36" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="8">
+        <v>33</v>
+      </c>
+      <c r="B37" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="8">
+        <v>34</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="8">
+        <v>35</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="8">
+        <v>36</v>
+      </c>
+      <c r="B40" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="8">
+        <v>37</v>
+      </c>
+      <c r="B41" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="8">
+        <v>38</v>
+      </c>
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="8">
+        <v>39</v>
+      </c>
+      <c r="B43" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="8">
+        <v>40</v>
+      </c>
+      <c r="B44" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="8">
+        <v>41</v>
+      </c>
+      <c r="B45" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="8">
+        <v>42</v>
+      </c>
+      <c r="B46" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="8">
+        <v>43</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="8">
+        <v>44</v>
+      </c>
+      <c r="B48" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="8">
+        <v>45</v>
+      </c>
+      <c r="B49" s="8">
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>